<commit_message>
Done with wdw replacement
</commit_message>
<xml_diff>
--- a/08.03.2023_Creative_QA_Report.xlsx
+++ b/08.03.2023_Creative_QA_Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\devsrv\Deezni Offers Macro\Disney_offers_macro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDB1B125-D05B-41C2-8A61-04B3CEC91752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{28DEF5A2-1FEE-406D-93DF-A481328DD4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="31920" xr2:uid="{1BA92678-42F0-477E-B029-6D69C005E10E}"/>
+    <workbookView xWindow="11925" yWindow="2775" windowWidth="43200" windowHeight="23445" xr2:uid="{83715349-9EF8-4D43-A5BB-727B0BBC63F9}"/>
   </bookViews>
   <sheets>
     <sheet name="GOOGLE DOCS HERE" sheetId="7" r:id="rId1"/>
@@ -9304,14 +9304,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C282CE-2DA7-450E-BF5D-099A65471D70}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36113C3-09C2-4429-A41B-CB7C6E4E589B}">
   <sheetPr codeName="Sheet1">
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:G1494"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P52" sqref="P52"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -43454,7 +43454,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246C42A9-C82B-4AA5-BC35-ADCD3993AD8F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E238D9B-551E-4D06-A3AD-0F45411A1445}">
   <sheetPr codeName="Sheet2">
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
@@ -55682,7 +55682,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A83F024-8442-43EB-85AD-807CA30FAFEB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D13DB0B-A405-495E-A449-F5BF5A5150B1}">
   <sheetPr codeName="Sheet4">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
@@ -55768,7 +55768,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A72FF2C-5901-4DAA-9348-2817647AE88B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1810BC-230D-4D93-BD8D-9B8DEB82E315}">
   <sheetPr codeName="Sheet5">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
@@ -55851,7 +55851,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C3491F-4995-4630-AD69-B15590ADD920}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8708EB00-47AD-4B01-84CF-81D3B9A259E0}">
   <sheetPr codeName="Sheet6">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
@@ -62481,7 +62481,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EAA59C0-E455-46E3-9058-17368F32B1B8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FC9868-2701-4A5F-9263-3A740CF5C90B}">
   <sheetPr codeName="Sheet7">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>

</xml_diff>